<commit_message>
Correct dates in results spreadsheet
</commit_message>
<xml_diff>
--- a/doc/Results.xlsx
+++ b/doc/Results.xlsx
@@ -488,7 +488,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,7 +644,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="n">
-        <v>42433</v>
+        <v>42432</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>19</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="n">
-        <v>42434</v>
+        <v>42432</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>20</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="n">
-        <v>42435</v>
+        <v>42432</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>20</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="n">
-        <v>42436</v>
+        <v>42432</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Change parameters and update results
</commit_message>
<xml_diff>
--- a/doc/Results.xlsx
+++ b/doc/Results.xlsx
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t xml:space="preserve">DATA</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t xml:space="preserve">511/1390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer=100*tanh+ 100*tanh  + 100 * sigmoid + softmax
+learning_rate=0,1
+n_stable=2
+n_iter=21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">505/1390</t>
   </si>
 </sst>
 </file>
@@ -377,20 +386,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -493,9 +494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>257040</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:colOff>256680</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -505,7 +506,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11694960" cy="9971640"/>
+          <a:ext cx="11534040" cy="9971280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -538,9 +539,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>257040</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:colOff>256680</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -550,7 +551,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11694960" cy="9971640"/>
+          <a:ext cx="11534040" cy="9971280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -583,9 +584,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>257040</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:colOff>256680</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -595,7 +596,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11694960" cy="9971640"/>
+          <a:ext cx="11534040" cy="9971280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -628,9 +629,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>257040</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:colOff>256680</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -640,7 +641,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11694960" cy="9971640"/>
+          <a:ext cx="11534040" cy="9971280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -673,9 +674,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>257040</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:colOff>256680</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -685,7 +686,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11694960" cy="9971640"/>
+          <a:ext cx="11534040" cy="9971280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -717,370 +718,402 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="36.8367346938775"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="36.4489795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="n">
+      <c r="A2" s="7" t="n">
         <v>42431</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11" t="n">
+      <c r="F2" s="8"/>
+      <c r="G2" s="9" t="n">
         <v>0.19799</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="H2" s="9" t="n">
         <v>2.65435</v>
       </c>
-      <c r="I2" s="11" t="n">
+      <c r="I2" s="9" t="n">
         <v>2.65656</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="11" t="n">
         <v>42432</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="0"/>
-      <c r="G3" s="15" t="n">
+      <c r="G3" s="13" t="n">
         <v>0.20771</v>
       </c>
-      <c r="H3" s="15" t="n">
+      <c r="H3" s="13" t="n">
         <v>2.64991</v>
       </c>
-      <c r="I3" s="15" t="n">
+      <c r="I3" s="13" t="n">
         <v>2.65093</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="n">
+      <c r="A4" s="11" t="n">
         <v>42432</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="0"/>
-      <c r="G4" s="15" t="n">
+      <c r="G4" s="13" t="n">
         <v>0.20775</v>
       </c>
-      <c r="H4" s="15" t="n">
+      <c r="H4" s="13" t="n">
         <v>2.64766</v>
       </c>
       <c r="I4" s="0"/>
       <c r="J4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="n">
+      <c r="A5" s="11" t="n">
         <v>42432</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="0"/>
-      <c r="G5" s="15" t="n">
+      <c r="G5" s="13" t="n">
         <v>0.20786</v>
       </c>
-      <c r="H5" s="15" t="n">
+      <c r="H5" s="13" t="n">
         <v>2.64963</v>
       </c>
       <c r="I5" s="0"/>
       <c r="J5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="n">
+      <c r="A6" s="11" t="n">
         <v>42432</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="0"/>
-      <c r="G6" s="15" t="n">
+      <c r="G6" s="13" t="n">
         <v>0.20764</v>
       </c>
-      <c r="H6" s="15" t="n">
+      <c r="H6" s="13" t="n">
         <v>2.64746</v>
       </c>
       <c r="I6" s="0"/>
       <c r="J6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="n">
+      <c r="A7" s="11" t="n">
         <v>42432</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="0"/>
-      <c r="G7" s="15" t="n">
+      <c r="G7" s="13" t="n">
         <v>0.20861</v>
       </c>
-      <c r="H7" s="15" t="n">
+      <c r="H7" s="13" t="n">
         <v>2.64754</v>
       </c>
       <c r="I7" s="0"/>
       <c r="J7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="n">
+      <c r="A8" s="11" t="n">
         <v>42432</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="0"/>
-      <c r="G8" s="15" t="n">
+      <c r="G8" s="13" t="n">
         <v>0.20843</v>
       </c>
-      <c r="H8" s="15" t="n">
+      <c r="H8" s="13" t="n">
         <v>2.64589</v>
       </c>
-      <c r="I8" s="15" t="n">
+      <c r="I8" s="13" t="n">
         <v>2.64736</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="n">
+      <c r="A9" s="11" t="n">
         <v>42432</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="0"/>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="0"/>
-      <c r="G9" s="15" t="n">
+      <c r="G9" s="13" t="n">
         <v>0.20559</v>
       </c>
-      <c r="H9" s="15" t="n">
+      <c r="H9" s="13" t="n">
         <v>2.66475</v>
       </c>
       <c r="I9" s="0"/>
       <c r="J9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="11" t="n">
         <v>42433</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="15" t="n">
+      <c r="G10" s="13" t="n">
         <v>0.2127</v>
       </c>
-      <c r="H10" s="15" t="n">
+      <c r="H10" s="13" t="n">
         <v>2.63403</v>
       </c>
-      <c r="I10" s="15" t="n">
+      <c r="I10" s="13" t="n">
         <v>2.64336</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="n">
+      <c r="A11" s="11" t="n">
         <v>42433</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="15" t="n">
+      <c r="G11" s="13" t="n">
         <v>0.22523</v>
       </c>
-      <c r="H11" s="15" t="n">
+      <c r="H11" s="13" t="n">
         <v>2.59278</v>
       </c>
-      <c r="I11" s="15" t="n">
+      <c r="I11" s="13" t="n">
         <v>2.7406</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="n">
+      <c r="A12" s="15" t="n">
         <v>42433</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="21" t="n">
+      <c r="G12" s="19" t="n">
         <v>0.23021</v>
       </c>
-      <c r="H12" s="21" t="n">
+      <c r="H12" s="19" t="n">
         <v>2.56315</v>
       </c>
-      <c r="I12" s="21" t="n">
+      <c r="I12" s="19" t="n">
         <v>2.56476</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="20" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="n">
+        <v>42433</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="19" t="n">
+        <v>0.23028</v>
+      </c>
+      <c r="H13" s="19" t="n">
+        <v>2.55942</v>
+      </c>
+      <c r="I13" s="19" t="n">
+        <v>2.56269</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>